<commit_message>
Game and Menu Flow update
Game screen added and game flow revised
</commit_message>
<xml_diff>
--- a/Game_Design/Transmission Ideas.xlsx
+++ b/Game_Design/Transmission Ideas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Transmission Ideas</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Auditive associations with huge interpretation value</t>
+  </si>
+  <si>
+    <t>Colours</t>
+  </si>
+  <si>
+    <t>Basic asoociation recogniceble patterns</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +494,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>